<commit_message>
test Decoder4To16 using full truth table
</commit_message>
<xml_diff>
--- a/src/test/resources/reference.xlsx
+++ b/src/test/resources/reference.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\code\cpu\circuit_sim_java\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A5A3EC-630C-4F0E-AF11-6155B0F42F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9633CC-93F6-4C1E-B958-7FED02836997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F7E82E32-581C-4D3D-B9D3-5EF07DB25AC1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F7E82E32-581C-4D3D-B9D3-5EF07DB25AC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Counter4" sheetId="1" r:id="rId1"/>
     <sheet name="DFlipFlop" sheetId="2" r:id="rId2"/>
+    <sheet name="Decoder4To16" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>CNT</t>
   </si>
@@ -67,6 +68,18 @@
   </si>
   <si>
     <t>nQ</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>EN1</t>
+  </si>
+  <si>
+    <t>EN2</t>
   </si>
 </sst>
 </file>
@@ -442,8 +455,8 @@
   <dimension ref="A1:K77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:F77"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +504,7 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:F18" si="0">IF(_xlfn.BITAND($K3,B$1)&gt;0,1,0)</f>
+        <f t="shared" ref="B3:E18" si="0">IF(_xlfn.BITAND($K3,B$1)&gt;0,1,0)</f>
         <v>1</v>
       </c>
       <c r="C3">
@@ -689,7 +702,7 @@
         <v>1</v>
       </c>
       <c r="K9">
-        <f t="shared" ref="K9:K40" si="4">K8-1</f>
+        <f t="shared" ref="K9" si="4">K8-1</f>
         <v>36</v>
       </c>
     </row>
@@ -749,7 +762,7 @@
         <v>1</v>
       </c>
       <c r="K11">
-        <f t="shared" ref="K11:K42" si="6">K10-1</f>
+        <f t="shared" ref="K11" si="6">K10-1</f>
         <v>38</v>
       </c>
     </row>
@@ -809,7 +822,7 @@
         <v>1</v>
       </c>
       <c r="K13">
-        <f t="shared" ref="K13:K44" si="8">K12-1</f>
+        <f t="shared" ref="K13" si="8">K12-1</f>
         <v>40</v>
       </c>
     </row>
@@ -869,7 +882,7 @@
         <v>1</v>
       </c>
       <c r="K15">
-        <f t="shared" ref="K15:K46" si="10">K14-1</f>
+        <f t="shared" ref="K15" si="10">K14-1</f>
         <v>42</v>
       </c>
     </row>
@@ -929,7 +942,7 @@
         <v>1</v>
       </c>
       <c r="K17">
-        <f t="shared" ref="K17:K48" si="12">K16-1</f>
+        <f t="shared" ref="K17" si="12">K16-1</f>
         <v>44</v>
       </c>
     </row>
@@ -989,7 +1002,7 @@
         <v>1</v>
       </c>
       <c r="K19">
-        <f t="shared" ref="K19:K50" si="14">K18-1</f>
+        <f t="shared" ref="K19" si="14">K18-1</f>
         <v>46</v>
       </c>
     </row>
@@ -1049,7 +1062,7 @@
         <v>0</v>
       </c>
       <c r="K21">
-        <f t="shared" ref="K21:K52" si="16">K20-1</f>
+        <f t="shared" ref="K21" si="16">K20-1</f>
         <v>48</v>
       </c>
     </row>
@@ -1109,7 +1122,7 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <f t="shared" ref="K23:K54" si="18">K22-1</f>
+        <f t="shared" ref="K23" si="18">K22-1</f>
         <v>50</v>
       </c>
     </row>
@@ -1169,7 +1182,7 @@
         <v>0</v>
       </c>
       <c r="K25">
-        <f t="shared" ref="K25:K56" si="20">K24-1</f>
+        <f t="shared" ref="K25" si="20">K24-1</f>
         <v>52</v>
       </c>
     </row>
@@ -1229,7 +1242,7 @@
         <v>0</v>
       </c>
       <c r="K27">
-        <f t="shared" ref="K27:K58" si="22">K26-1</f>
+        <f t="shared" ref="K27" si="22">K26-1</f>
         <v>54</v>
       </c>
     </row>
@@ -1289,7 +1302,7 @@
         <v>0</v>
       </c>
       <c r="K29">
-        <f t="shared" ref="K29:K60" si="24">K28-1</f>
+        <f t="shared" ref="K29" si="24">K28-1</f>
         <v>56</v>
       </c>
     </row>
@@ -1349,7 +1362,7 @@
         <v>0</v>
       </c>
       <c r="K31">
-        <f t="shared" ref="K31:K77" si="26">K30-1</f>
+        <f t="shared" ref="K31" si="26">K30-1</f>
         <v>58</v>
       </c>
     </row>
@@ -1409,7 +1422,7 @@
         <v>0</v>
       </c>
       <c r="K33">
-        <f t="shared" ref="K33:K77" si="28">K32-1</f>
+        <f t="shared" ref="K33" si="28">K32-1</f>
         <v>60</v>
       </c>
     </row>
@@ -1469,13 +1482,13 @@
         <v>0</v>
       </c>
       <c r="K35">
-        <f t="shared" ref="K35:K77" si="30">K34-1</f>
+        <f t="shared" ref="K35" si="30">K34-1</f>
         <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" ref="A36:E78" si="31">IF(_xlfn.BITAND($K36,A$1)&gt;0,1,0)</f>
+        <f t="shared" ref="A36:E77" si="31">IF(_xlfn.BITAND($K36,A$1)&gt;0,1,0)</f>
         <v>1</v>
       </c>
       <c r="B36">
@@ -1529,7 +1542,7 @@
         <v>1</v>
       </c>
       <c r="K37">
-        <f t="shared" ref="K37:K77" si="33">K36-1</f>
+        <f t="shared" ref="K37" si="33">K36-1</f>
         <v>64</v>
       </c>
     </row>
@@ -1589,7 +1602,7 @@
         <v>1</v>
       </c>
       <c r="K39">
-        <f t="shared" ref="K39:K77" si="35">K38-1</f>
+        <f t="shared" ref="K39" si="35">K38-1</f>
         <v>66</v>
       </c>
     </row>
@@ -1649,7 +1662,7 @@
         <v>1</v>
       </c>
       <c r="K41">
-        <f t="shared" ref="K41:K77" si="37">K40-1</f>
+        <f t="shared" ref="K41" si="37">K40-1</f>
         <v>68</v>
       </c>
     </row>
@@ -1709,7 +1722,7 @@
         <v>1</v>
       </c>
       <c r="K43">
-        <f t="shared" ref="K43:K77" si="39">K42-1</f>
+        <f t="shared" ref="K43" si="39">K42-1</f>
         <v>70</v>
       </c>
     </row>
@@ -1769,7 +1782,7 @@
         <v>1</v>
       </c>
       <c r="K45">
-        <f t="shared" ref="K45:K77" si="41">K44-1</f>
+        <f t="shared" ref="K45" si="41">K44-1</f>
         <v>72</v>
       </c>
     </row>
@@ -1829,7 +1842,7 @@
         <v>1</v>
       </c>
       <c r="K47">
-        <f t="shared" ref="K47:K77" si="43">K46-1</f>
+        <f t="shared" ref="K47" si="43">K46-1</f>
         <v>74</v>
       </c>
     </row>
@@ -1889,7 +1902,7 @@
         <v>1</v>
       </c>
       <c r="K49">
-        <f t="shared" ref="K49:K77" si="45">K48-1</f>
+        <f t="shared" ref="K49" si="45">K48-1</f>
         <v>76</v>
       </c>
     </row>
@@ -1949,7 +1962,7 @@
         <v>1</v>
       </c>
       <c r="K51">
-        <f t="shared" ref="K51:K77" si="47">K50-1</f>
+        <f t="shared" ref="K51" si="47">K50-1</f>
         <v>78</v>
       </c>
     </row>
@@ -2009,7 +2022,7 @@
         <v>0</v>
       </c>
       <c r="K53">
-        <f t="shared" ref="K53:K77" si="49">K52-1</f>
+        <f t="shared" ref="K53" si="49">K52-1</f>
         <v>80</v>
       </c>
     </row>
@@ -2069,7 +2082,7 @@
         <v>0</v>
       </c>
       <c r="K55">
-        <f t="shared" ref="K55:K77" si="51">K54-1</f>
+        <f t="shared" ref="K55" si="51">K54-1</f>
         <v>82</v>
       </c>
     </row>
@@ -2129,7 +2142,7 @@
         <v>0</v>
       </c>
       <c r="K57">
-        <f t="shared" ref="K57:K77" si="53">K56-1</f>
+        <f t="shared" ref="K57" si="53">K56-1</f>
         <v>84</v>
       </c>
     </row>
@@ -2189,7 +2202,7 @@
         <v>0</v>
       </c>
       <c r="K59">
-        <f t="shared" ref="K59:K77" si="55">K58-1</f>
+        <f t="shared" ref="K59" si="55">K58-1</f>
         <v>86</v>
       </c>
     </row>
@@ -2249,7 +2262,7 @@
         <v>0</v>
       </c>
       <c r="K61">
-        <f t="shared" ref="K61:K77" si="57">K60-1</f>
+        <f t="shared" ref="K61" si="57">K60-1</f>
         <v>88</v>
       </c>
     </row>
@@ -2309,7 +2322,7 @@
         <v>0</v>
       </c>
       <c r="K63">
-        <f t="shared" ref="K63:K77" si="59">K62-1</f>
+        <f t="shared" ref="K63" si="59">K62-1</f>
         <v>90</v>
       </c>
     </row>
@@ -2369,7 +2382,7 @@
         <v>0</v>
       </c>
       <c r="K65">
-        <f t="shared" ref="K65:K77" si="61">K64-1</f>
+        <f t="shared" ref="K65" si="61">K64-1</f>
         <v>92</v>
       </c>
     </row>
@@ -2429,7 +2442,7 @@
         <v>0</v>
       </c>
       <c r="K67">
-        <f t="shared" ref="K67:K77" si="63">K66-1</f>
+        <f t="shared" ref="K67" si="63">K66-1</f>
         <v>94</v>
       </c>
     </row>
@@ -2455,7 +2468,7 @@
         <v>0</v>
       </c>
       <c r="F68">
-        <f t="shared" ref="F68:F78" si="64">IF(E68=0,1,0)</f>
+        <f t="shared" ref="F68:F77" si="64">IF(E68=0,1,0)</f>
         <v>1</v>
       </c>
       <c r="K68">
@@ -2489,7 +2502,7 @@
         <v>1</v>
       </c>
       <c r="K69">
-        <f t="shared" ref="K69:K77" si="66">K68-1</f>
+        <f t="shared" ref="K69" si="66">K68-1</f>
         <v>96</v>
       </c>
     </row>
@@ -2549,7 +2562,7 @@
         <v>1</v>
       </c>
       <c r="K71">
-        <f t="shared" ref="K71:K77" si="68">K70-1</f>
+        <f t="shared" ref="K71" si="68">K70-1</f>
         <v>98</v>
       </c>
     </row>
@@ -2609,7 +2622,7 @@
         <v>1</v>
       </c>
       <c r="K73">
-        <f t="shared" ref="K73:K77" si="70">K72-1</f>
+        <f t="shared" ref="K73" si="70">K72-1</f>
         <v>100</v>
       </c>
     </row>
@@ -2669,7 +2682,7 @@
         <v>1</v>
       </c>
       <c r="K75">
-        <f t="shared" ref="K75:K77" si="72">K74-1</f>
+        <f t="shared" ref="K75" si="72">K74-1</f>
         <v>102</v>
       </c>
     </row>
@@ -2745,8 +2758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40BB848D-3229-44FC-98DC-09C2BB5C1F8C}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2880,4 +2893,4440 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECA2E51-2723-4078-B266-B13DFD3B37AF}">
+  <dimension ref="A2:V66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2">
+        <v>5</v>
+      </c>
+      <c r="M2">
+        <v>6</v>
+      </c>
+      <c r="N2">
+        <v>7</v>
+      </c>
+      <c r="O2">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>9</v>
+      </c>
+      <c r="Q2">
+        <v>10</v>
+      </c>
+      <c r="R2">
+        <v>11</v>
+      </c>
+      <c r="S2">
+        <v>12</v>
+      </c>
+      <c r="T2">
+        <v>13</v>
+      </c>
+      <c r="U2">
+        <v>14</v>
+      </c>
+      <c r="V2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="V9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <v>1</v>
+      </c>
+      <c r="V11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>1</v>
+      </c>
+      <c r="U13">
+        <v>1</v>
+      </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>1</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+      <c r="U18">
+        <v>1</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>1</v>
+      </c>
+      <c r="U19">
+        <v>1</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <v>1</v>
+      </c>
+      <c r="U20">
+        <v>1</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>1</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="V21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="T22">
+        <v>1</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="V22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23">
+        <v>1</v>
+      </c>
+      <c r="S23">
+        <v>1</v>
+      </c>
+      <c r="T23">
+        <v>1</v>
+      </c>
+      <c r="U23">
+        <v>1</v>
+      </c>
+      <c r="V23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="R24">
+        <v>1</v>
+      </c>
+      <c r="S24">
+        <v>1</v>
+      </c>
+      <c r="T24">
+        <v>1</v>
+      </c>
+      <c r="U24">
+        <v>1</v>
+      </c>
+      <c r="V24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+      <c r="R25">
+        <v>1</v>
+      </c>
+      <c r="S25">
+        <v>1</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="U25">
+        <v>1</v>
+      </c>
+      <c r="V25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+      <c r="S26">
+        <v>1</v>
+      </c>
+      <c r="T26">
+        <v>1</v>
+      </c>
+      <c r="U26">
+        <v>1</v>
+      </c>
+      <c r="V26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+      <c r="R27">
+        <v>1</v>
+      </c>
+      <c r="S27">
+        <v>1</v>
+      </c>
+      <c r="T27">
+        <v>1</v>
+      </c>
+      <c r="U27">
+        <v>1</v>
+      </c>
+      <c r="V27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+      <c r="R28">
+        <v>1</v>
+      </c>
+      <c r="S28">
+        <v>1</v>
+      </c>
+      <c r="T28">
+        <v>1</v>
+      </c>
+      <c r="U28">
+        <v>1</v>
+      </c>
+      <c r="V28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <v>1</v>
+      </c>
+      <c r="R29">
+        <v>1</v>
+      </c>
+      <c r="S29">
+        <v>1</v>
+      </c>
+      <c r="T29">
+        <v>1</v>
+      </c>
+      <c r="U29">
+        <v>1</v>
+      </c>
+      <c r="V29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+      <c r="O30">
+        <v>1</v>
+      </c>
+      <c r="P30">
+        <v>1</v>
+      </c>
+      <c r="Q30">
+        <v>1</v>
+      </c>
+      <c r="R30">
+        <v>1</v>
+      </c>
+      <c r="S30">
+        <v>1</v>
+      </c>
+      <c r="T30">
+        <v>1</v>
+      </c>
+      <c r="U30">
+        <v>1</v>
+      </c>
+      <c r="V30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="Q31">
+        <v>1</v>
+      </c>
+      <c r="R31">
+        <v>1</v>
+      </c>
+      <c r="S31">
+        <v>1</v>
+      </c>
+      <c r="T31">
+        <v>1</v>
+      </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
+      <c r="V31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32">
+        <v>1</v>
+      </c>
+      <c r="Q32">
+        <v>1</v>
+      </c>
+      <c r="R32">
+        <v>1</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
+      </c>
+      <c r="T32">
+        <v>1</v>
+      </c>
+      <c r="U32">
+        <v>1</v>
+      </c>
+      <c r="V32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
+      <c r="O33">
+        <v>1</v>
+      </c>
+      <c r="P33">
+        <v>1</v>
+      </c>
+      <c r="Q33">
+        <v>1</v>
+      </c>
+      <c r="R33">
+        <v>1</v>
+      </c>
+      <c r="S33">
+        <v>1</v>
+      </c>
+      <c r="T33">
+        <v>1</v>
+      </c>
+      <c r="U33">
+        <v>1</v>
+      </c>
+      <c r="V33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>1</v>
+      </c>
+      <c r="P34">
+        <v>1</v>
+      </c>
+      <c r="Q34">
+        <v>1</v>
+      </c>
+      <c r="R34">
+        <v>1</v>
+      </c>
+      <c r="S34">
+        <v>1</v>
+      </c>
+      <c r="T34">
+        <v>1</v>
+      </c>
+      <c r="U34">
+        <v>1</v>
+      </c>
+      <c r="V34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
+      <c r="P35">
+        <v>1</v>
+      </c>
+      <c r="Q35">
+        <v>1</v>
+      </c>
+      <c r="R35">
+        <v>1</v>
+      </c>
+      <c r="S35">
+        <v>1</v>
+      </c>
+      <c r="T35">
+        <v>1</v>
+      </c>
+      <c r="U35">
+        <v>1</v>
+      </c>
+      <c r="V35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36">
+        <v>1</v>
+      </c>
+      <c r="P36">
+        <v>1</v>
+      </c>
+      <c r="Q36">
+        <v>1</v>
+      </c>
+      <c r="R36">
+        <v>1</v>
+      </c>
+      <c r="S36">
+        <v>1</v>
+      </c>
+      <c r="T36">
+        <v>1</v>
+      </c>
+      <c r="U36">
+        <v>1</v>
+      </c>
+      <c r="V36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
+      <c r="O37">
+        <v>1</v>
+      </c>
+      <c r="P37">
+        <v>1</v>
+      </c>
+      <c r="Q37">
+        <v>1</v>
+      </c>
+      <c r="R37">
+        <v>1</v>
+      </c>
+      <c r="S37">
+        <v>1</v>
+      </c>
+      <c r="T37">
+        <v>1</v>
+      </c>
+      <c r="U37">
+        <v>1</v>
+      </c>
+      <c r="V37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <v>1</v>
+      </c>
+      <c r="O38">
+        <v>1</v>
+      </c>
+      <c r="P38">
+        <v>1</v>
+      </c>
+      <c r="Q38">
+        <v>1</v>
+      </c>
+      <c r="R38">
+        <v>1</v>
+      </c>
+      <c r="S38">
+        <v>1</v>
+      </c>
+      <c r="T38">
+        <v>1</v>
+      </c>
+      <c r="U38">
+        <v>1</v>
+      </c>
+      <c r="V38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <v>1</v>
+      </c>
+      <c r="O39">
+        <v>1</v>
+      </c>
+      <c r="P39">
+        <v>1</v>
+      </c>
+      <c r="Q39">
+        <v>1</v>
+      </c>
+      <c r="R39">
+        <v>1</v>
+      </c>
+      <c r="S39">
+        <v>1</v>
+      </c>
+      <c r="T39">
+        <v>1</v>
+      </c>
+      <c r="U39">
+        <v>1</v>
+      </c>
+      <c r="V39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>1</v>
+      </c>
+      <c r="O40">
+        <v>1</v>
+      </c>
+      <c r="P40">
+        <v>1</v>
+      </c>
+      <c r="Q40">
+        <v>1</v>
+      </c>
+      <c r="R40">
+        <v>1</v>
+      </c>
+      <c r="S40">
+        <v>1</v>
+      </c>
+      <c r="T40">
+        <v>1</v>
+      </c>
+      <c r="U40">
+        <v>1</v>
+      </c>
+      <c r="V40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="N41">
+        <v>1</v>
+      </c>
+      <c r="O41">
+        <v>1</v>
+      </c>
+      <c r="P41">
+        <v>1</v>
+      </c>
+      <c r="Q41">
+        <v>1</v>
+      </c>
+      <c r="R41">
+        <v>1</v>
+      </c>
+      <c r="S41">
+        <v>1</v>
+      </c>
+      <c r="T41">
+        <v>1</v>
+      </c>
+      <c r="U41">
+        <v>1</v>
+      </c>
+      <c r="V41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>1</v>
+      </c>
+      <c r="O42">
+        <v>1</v>
+      </c>
+      <c r="P42">
+        <v>1</v>
+      </c>
+      <c r="Q42">
+        <v>1</v>
+      </c>
+      <c r="R42">
+        <v>1</v>
+      </c>
+      <c r="S42">
+        <v>1</v>
+      </c>
+      <c r="T42">
+        <v>1</v>
+      </c>
+      <c r="U42">
+        <v>1</v>
+      </c>
+      <c r="V42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+      <c r="N43">
+        <v>1</v>
+      </c>
+      <c r="O43">
+        <v>1</v>
+      </c>
+      <c r="P43">
+        <v>1</v>
+      </c>
+      <c r="Q43">
+        <v>1</v>
+      </c>
+      <c r="R43">
+        <v>1</v>
+      </c>
+      <c r="S43">
+        <v>1</v>
+      </c>
+      <c r="T43">
+        <v>1</v>
+      </c>
+      <c r="U43">
+        <v>1</v>
+      </c>
+      <c r="V43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <v>1</v>
+      </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+      <c r="N44">
+        <v>1</v>
+      </c>
+      <c r="O44">
+        <v>1</v>
+      </c>
+      <c r="P44">
+        <v>1</v>
+      </c>
+      <c r="Q44">
+        <v>1</v>
+      </c>
+      <c r="R44">
+        <v>1</v>
+      </c>
+      <c r="S44">
+        <v>1</v>
+      </c>
+      <c r="T44">
+        <v>1</v>
+      </c>
+      <c r="U44">
+        <v>1</v>
+      </c>
+      <c r="V44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>0</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+      <c r="L45">
+        <v>1</v>
+      </c>
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <v>1</v>
+      </c>
+      <c r="O45">
+        <v>1</v>
+      </c>
+      <c r="P45">
+        <v>1</v>
+      </c>
+      <c r="Q45">
+        <v>1</v>
+      </c>
+      <c r="R45">
+        <v>1</v>
+      </c>
+      <c r="S45">
+        <v>1</v>
+      </c>
+      <c r="T45">
+        <v>1</v>
+      </c>
+      <c r="U45">
+        <v>1</v>
+      </c>
+      <c r="V45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="L46">
+        <v>1</v>
+      </c>
+      <c r="M46">
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <v>1</v>
+      </c>
+      <c r="O46">
+        <v>1</v>
+      </c>
+      <c r="P46">
+        <v>1</v>
+      </c>
+      <c r="Q46">
+        <v>1</v>
+      </c>
+      <c r="R46">
+        <v>1</v>
+      </c>
+      <c r="S46">
+        <v>1</v>
+      </c>
+      <c r="T46">
+        <v>1</v>
+      </c>
+      <c r="U46">
+        <v>1</v>
+      </c>
+      <c r="V46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>0</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+      <c r="L47">
+        <v>1</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
+      <c r="O47">
+        <v>1</v>
+      </c>
+      <c r="P47">
+        <v>1</v>
+      </c>
+      <c r="Q47">
+        <v>1</v>
+      </c>
+      <c r="R47">
+        <v>1</v>
+      </c>
+      <c r="S47">
+        <v>1</v>
+      </c>
+      <c r="T47">
+        <v>1</v>
+      </c>
+      <c r="U47">
+        <v>1</v>
+      </c>
+      <c r="V47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="L48">
+        <v>1</v>
+      </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <v>1</v>
+      </c>
+      <c r="O48">
+        <v>1</v>
+      </c>
+      <c r="P48">
+        <v>1</v>
+      </c>
+      <c r="Q48">
+        <v>1</v>
+      </c>
+      <c r="R48">
+        <v>1</v>
+      </c>
+      <c r="S48">
+        <v>1</v>
+      </c>
+      <c r="T48">
+        <v>1</v>
+      </c>
+      <c r="U48">
+        <v>1</v>
+      </c>
+      <c r="V48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>0</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
+      <c r="L49">
+        <v>1</v>
+      </c>
+      <c r="M49">
+        <v>1</v>
+      </c>
+      <c r="N49">
+        <v>1</v>
+      </c>
+      <c r="O49">
+        <v>1</v>
+      </c>
+      <c r="P49">
+        <v>1</v>
+      </c>
+      <c r="Q49">
+        <v>1</v>
+      </c>
+      <c r="R49">
+        <v>1</v>
+      </c>
+      <c r="S49">
+        <v>1</v>
+      </c>
+      <c r="T49">
+        <v>1</v>
+      </c>
+      <c r="U49">
+        <v>1</v>
+      </c>
+      <c r="V49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="M50">
+        <v>1</v>
+      </c>
+      <c r="N50">
+        <v>1</v>
+      </c>
+      <c r="O50">
+        <v>1</v>
+      </c>
+      <c r="P50">
+        <v>1</v>
+      </c>
+      <c r="Q50">
+        <v>1</v>
+      </c>
+      <c r="R50">
+        <v>1</v>
+      </c>
+      <c r="S50">
+        <v>1</v>
+      </c>
+      <c r="T50">
+        <v>1</v>
+      </c>
+      <c r="U50">
+        <v>1</v>
+      </c>
+      <c r="V50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>0</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+      <c r="K51">
+        <v>1</v>
+      </c>
+      <c r="L51">
+        <v>1</v>
+      </c>
+      <c r="M51">
+        <v>1</v>
+      </c>
+      <c r="N51">
+        <v>1</v>
+      </c>
+      <c r="O51">
+        <v>1</v>
+      </c>
+      <c r="P51">
+        <v>1</v>
+      </c>
+      <c r="Q51">
+        <v>1</v>
+      </c>
+      <c r="R51">
+        <v>1</v>
+      </c>
+      <c r="S51">
+        <v>1</v>
+      </c>
+      <c r="T51">
+        <v>1</v>
+      </c>
+      <c r="U51">
+        <v>1</v>
+      </c>
+      <c r="V51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
+      <c r="K52">
+        <v>1</v>
+      </c>
+      <c r="L52">
+        <v>1</v>
+      </c>
+      <c r="M52">
+        <v>1</v>
+      </c>
+      <c r="N52">
+        <v>1</v>
+      </c>
+      <c r="O52">
+        <v>1</v>
+      </c>
+      <c r="P52">
+        <v>1</v>
+      </c>
+      <c r="Q52">
+        <v>1</v>
+      </c>
+      <c r="R52">
+        <v>1</v>
+      </c>
+      <c r="S52">
+        <v>1</v>
+      </c>
+      <c r="T52">
+        <v>1</v>
+      </c>
+      <c r="U52">
+        <v>1</v>
+      </c>
+      <c r="V52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>0</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="K53">
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <v>1</v>
+      </c>
+      <c r="M53">
+        <v>1</v>
+      </c>
+      <c r="N53">
+        <v>1</v>
+      </c>
+      <c r="O53">
+        <v>1</v>
+      </c>
+      <c r="P53">
+        <v>1</v>
+      </c>
+      <c r="Q53">
+        <v>1</v>
+      </c>
+      <c r="R53">
+        <v>1</v>
+      </c>
+      <c r="S53">
+        <v>1</v>
+      </c>
+      <c r="T53">
+        <v>1</v>
+      </c>
+      <c r="U53">
+        <v>1</v>
+      </c>
+      <c r="V53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <v>1</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+      <c r="L54">
+        <v>1</v>
+      </c>
+      <c r="M54">
+        <v>1</v>
+      </c>
+      <c r="N54">
+        <v>1</v>
+      </c>
+      <c r="O54">
+        <v>1</v>
+      </c>
+      <c r="P54">
+        <v>1</v>
+      </c>
+      <c r="Q54">
+        <v>1</v>
+      </c>
+      <c r="R54">
+        <v>1</v>
+      </c>
+      <c r="S54">
+        <v>1</v>
+      </c>
+      <c r="T54">
+        <v>1</v>
+      </c>
+      <c r="U54">
+        <v>1</v>
+      </c>
+      <c r="V54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>0</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
+      </c>
+      <c r="J55">
+        <v>1</v>
+      </c>
+      <c r="K55">
+        <v>1</v>
+      </c>
+      <c r="L55">
+        <v>1</v>
+      </c>
+      <c r="M55">
+        <v>1</v>
+      </c>
+      <c r="N55">
+        <v>1</v>
+      </c>
+      <c r="O55">
+        <v>1</v>
+      </c>
+      <c r="P55">
+        <v>1</v>
+      </c>
+      <c r="Q55">
+        <v>1</v>
+      </c>
+      <c r="R55">
+        <v>1</v>
+      </c>
+      <c r="S55">
+        <v>1</v>
+      </c>
+      <c r="T55">
+        <v>1</v>
+      </c>
+      <c r="U55">
+        <v>1</v>
+      </c>
+      <c r="V55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="K56">
+        <v>1</v>
+      </c>
+      <c r="L56">
+        <v>1</v>
+      </c>
+      <c r="M56">
+        <v>1</v>
+      </c>
+      <c r="N56">
+        <v>1</v>
+      </c>
+      <c r="O56">
+        <v>1</v>
+      </c>
+      <c r="P56">
+        <v>1</v>
+      </c>
+      <c r="Q56">
+        <v>1</v>
+      </c>
+      <c r="R56">
+        <v>1</v>
+      </c>
+      <c r="S56">
+        <v>1</v>
+      </c>
+      <c r="T56">
+        <v>1</v>
+      </c>
+      <c r="U56">
+        <v>1</v>
+      </c>
+      <c r="V56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>0</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+      <c r="L57">
+        <v>1</v>
+      </c>
+      <c r="M57">
+        <v>1</v>
+      </c>
+      <c r="N57">
+        <v>1</v>
+      </c>
+      <c r="O57">
+        <v>1</v>
+      </c>
+      <c r="P57">
+        <v>1</v>
+      </c>
+      <c r="Q57">
+        <v>1</v>
+      </c>
+      <c r="R57">
+        <v>1</v>
+      </c>
+      <c r="S57">
+        <v>1</v>
+      </c>
+      <c r="T57">
+        <v>1</v>
+      </c>
+      <c r="U57">
+        <v>1</v>
+      </c>
+      <c r="V57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="L58">
+        <v>1</v>
+      </c>
+      <c r="M58">
+        <v>1</v>
+      </c>
+      <c r="N58">
+        <v>1</v>
+      </c>
+      <c r="O58">
+        <v>1</v>
+      </c>
+      <c r="P58">
+        <v>1</v>
+      </c>
+      <c r="Q58">
+        <v>1</v>
+      </c>
+      <c r="R58">
+        <v>1</v>
+      </c>
+      <c r="S58">
+        <v>1</v>
+      </c>
+      <c r="T58">
+        <v>1</v>
+      </c>
+      <c r="U58">
+        <v>1</v>
+      </c>
+      <c r="V58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>0</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+      <c r="K59">
+        <v>1</v>
+      </c>
+      <c r="L59">
+        <v>1</v>
+      </c>
+      <c r="M59">
+        <v>1</v>
+      </c>
+      <c r="N59">
+        <v>1</v>
+      </c>
+      <c r="O59">
+        <v>1</v>
+      </c>
+      <c r="P59">
+        <v>1</v>
+      </c>
+      <c r="Q59">
+        <v>1</v>
+      </c>
+      <c r="R59">
+        <v>1</v>
+      </c>
+      <c r="S59">
+        <v>1</v>
+      </c>
+      <c r="T59">
+        <v>1</v>
+      </c>
+      <c r="U59">
+        <v>1</v>
+      </c>
+      <c r="V59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>1</v>
+      </c>
+      <c r="K60">
+        <v>1</v>
+      </c>
+      <c r="L60">
+        <v>1</v>
+      </c>
+      <c r="M60">
+        <v>1</v>
+      </c>
+      <c r="N60">
+        <v>1</v>
+      </c>
+      <c r="O60">
+        <v>1</v>
+      </c>
+      <c r="P60">
+        <v>1</v>
+      </c>
+      <c r="Q60">
+        <v>1</v>
+      </c>
+      <c r="R60">
+        <v>1</v>
+      </c>
+      <c r="S60">
+        <v>1</v>
+      </c>
+      <c r="T60">
+        <v>1</v>
+      </c>
+      <c r="U60">
+        <v>1</v>
+      </c>
+      <c r="V60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>0</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <v>1</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+      <c r="K61">
+        <v>1</v>
+      </c>
+      <c r="L61">
+        <v>1</v>
+      </c>
+      <c r="M61">
+        <v>1</v>
+      </c>
+      <c r="N61">
+        <v>1</v>
+      </c>
+      <c r="O61">
+        <v>1</v>
+      </c>
+      <c r="P61">
+        <v>1</v>
+      </c>
+      <c r="Q61">
+        <v>1</v>
+      </c>
+      <c r="R61">
+        <v>1</v>
+      </c>
+      <c r="S61">
+        <v>1</v>
+      </c>
+      <c r="T61">
+        <v>1</v>
+      </c>
+      <c r="U61">
+        <v>1</v>
+      </c>
+      <c r="V61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+      <c r="K62">
+        <v>1</v>
+      </c>
+      <c r="L62">
+        <v>1</v>
+      </c>
+      <c r="M62">
+        <v>1</v>
+      </c>
+      <c r="N62">
+        <v>1</v>
+      </c>
+      <c r="O62">
+        <v>1</v>
+      </c>
+      <c r="P62">
+        <v>1</v>
+      </c>
+      <c r="Q62">
+        <v>1</v>
+      </c>
+      <c r="R62">
+        <v>1</v>
+      </c>
+      <c r="S62">
+        <v>1</v>
+      </c>
+      <c r="T62">
+        <v>1</v>
+      </c>
+      <c r="U62">
+        <v>1</v>
+      </c>
+      <c r="V62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>0</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="I63">
+        <v>1</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
+      <c r="L63">
+        <v>1</v>
+      </c>
+      <c r="M63">
+        <v>1</v>
+      </c>
+      <c r="N63">
+        <v>1</v>
+      </c>
+      <c r="O63">
+        <v>1</v>
+      </c>
+      <c r="P63">
+        <v>1</v>
+      </c>
+      <c r="Q63">
+        <v>1</v>
+      </c>
+      <c r="R63">
+        <v>1</v>
+      </c>
+      <c r="S63">
+        <v>1</v>
+      </c>
+      <c r="T63">
+        <v>1</v>
+      </c>
+      <c r="U63">
+        <v>1</v>
+      </c>
+      <c r="V63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="J64">
+        <v>1</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+      <c r="L64">
+        <v>1</v>
+      </c>
+      <c r="M64">
+        <v>1</v>
+      </c>
+      <c r="N64">
+        <v>1</v>
+      </c>
+      <c r="O64">
+        <v>1</v>
+      </c>
+      <c r="P64">
+        <v>1</v>
+      </c>
+      <c r="Q64">
+        <v>1</v>
+      </c>
+      <c r="R64">
+        <v>1</v>
+      </c>
+      <c r="S64">
+        <v>1</v>
+      </c>
+      <c r="T64">
+        <v>1</v>
+      </c>
+      <c r="U64">
+        <v>1</v>
+      </c>
+      <c r="V64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>0</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65">
+        <v>1</v>
+      </c>
+      <c r="J65">
+        <v>1</v>
+      </c>
+      <c r="K65">
+        <v>1</v>
+      </c>
+      <c r="L65">
+        <v>1</v>
+      </c>
+      <c r="M65">
+        <v>1</v>
+      </c>
+      <c r="N65">
+        <v>1</v>
+      </c>
+      <c r="O65">
+        <v>1</v>
+      </c>
+      <c r="P65">
+        <v>1</v>
+      </c>
+      <c r="Q65">
+        <v>1</v>
+      </c>
+      <c r="R65">
+        <v>1</v>
+      </c>
+      <c r="S65">
+        <v>1</v>
+      </c>
+      <c r="T65">
+        <v>1</v>
+      </c>
+      <c r="U65">
+        <v>1</v>
+      </c>
+      <c r="V65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>1</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66">
+        <v>1</v>
+      </c>
+      <c r="J66">
+        <v>1</v>
+      </c>
+      <c r="K66">
+        <v>1</v>
+      </c>
+      <c r="L66">
+        <v>1</v>
+      </c>
+      <c r="M66">
+        <v>1</v>
+      </c>
+      <c r="N66">
+        <v>1</v>
+      </c>
+      <c r="O66">
+        <v>1</v>
+      </c>
+      <c r="P66">
+        <v>1</v>
+      </c>
+      <c r="Q66">
+        <v>1</v>
+      </c>
+      <c r="R66">
+        <v>1</v>
+      </c>
+      <c r="S66">
+        <v>1</v>
+      </c>
+      <c r="T66">
+        <v>1</v>
+      </c>
+      <c r="U66">
+        <v>1</v>
+      </c>
+      <c r="V66">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>